<commit_message>
Updated BOM, schematic and PCB
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t xml:space="preserve">LCSC Part Number</t>
   </si>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">HTC Korea TAEJIN Tech</t>
   </si>
   <si>
-    <t xml:space="preserve">SOP-8</t>
+    <t xml:space="preserve">DIP-8</t>
   </si>
   <si>
     <t xml:space="preserve">RS-485 ICs SOP-8 RoHS</t>
@@ -233,6 +233,21 @@
   </si>
   <si>
     <t xml:space="preserve">XLR 5 pin female connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C430283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI8660AB-B-IS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicon Labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOIC-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 channel optical isolator</t>
   </si>
 </sst>
 </file>
@@ -341,15 +356,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.14"/>
@@ -686,10 +701,30 @@
         <v>2</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Updated PCB, schematic and BOM to be current and look neat and tidy
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t xml:space="preserve">LCSC Part Number</t>
   </si>
@@ -184,21 +184,6 @@
     <t xml:space="preserve">High Precision &amp; Low TCR SMD Resistors 10KOhms ±0.1% 1/4W 1206 RoHS</t>
   </si>
   <si>
-    <t xml:space="preserve">C357757</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0201X6S104K6R3NTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EYANG(Shenzhen Eyang Tech Development)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 100nF 6.3V 0201 RoHS</t>
-  </si>
-  <si>
     <t xml:space="preserve">C481667</t>
   </si>
   <si>
@@ -248,6 +233,51 @@
   </si>
   <si>
     <t xml:space="preserve">6 channel optical isolator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C433729</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD 1/4W 330R J T/B A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330 ohm tht resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C142297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6n137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everlight Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6n137 optical isolator IC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C568944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HL-508H256WC-HD_6000K_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HONGLITRONIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED (assorted colours recommended)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FS10UM-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitsubishi Electric Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High switching frequency NPN mosfet</t>
   </si>
 </sst>
 </file>
@@ -330,13 +360,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -356,15 +394,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.14"/>
@@ -598,7 +636,7 @@
         <v>49</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -638,7 +676,7 @@
         <v>58</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +696,7 @@
         <v>63</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -666,30 +704,30 @@
         <v>64</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="F15" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>69</v>
@@ -698,29 +736,90 @@
         <v>70</v>
       </c>
       <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>